<commit_message>
MVP Product Backlog updated...
21/10/2021
</commit_message>
<xml_diff>
--- a/ITProjectManagement/BA/SpecsWireframes/MVP/005MVPProductBacklog.xlsx
+++ b/ITProjectManagement/BA/SpecsWireframes/MVP/005MVPProductBacklog.xlsx
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="152">
   <si>
     <t>Anodiam</t>
   </si>
@@ -415,30 +415,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> as a student with anodiam.com</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fill up all the (mandatory) fields in the registration section of the Student Registration Page and click on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Register </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>button.</t>
     </r>
   </si>
   <si>
@@ -3103,7 +3079,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> I click on the </t>
+      <t xml:space="preserve"> I fill up all the fields: (username, password, email) (all mandatory) in the registration section of the Student Registration Page and click on the </t>
     </r>
     <r>
       <rPr>
@@ -3147,6 +3123,105 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Fill up all the fields: (username, password, email) (all mandatory) with valid informations in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>button.</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter invalid username
+(Less than 8 characters long)
+in the registration section of the Student Registration Page and click on the Register button..</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Username cannot be less than 8 characters</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Username already exists</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="10"/>
@@ -3163,6 +3238,656 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter  invalid username (Less than 8 characters long or 
+an already existing username) in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button on the student registration page of anodiam.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Username cannot be less than 8 characters long</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter  invalid username (Less than 8 characters long or 
+an already existing username) in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button on the student registration page of anodiam.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Username already exists.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Invalid password. Password must be 8 to 20 characters long, must not contain your username and must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character (!, @, #, $, %, ^, &amp;, *, £)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter invalid password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Less than 8 characters or more than 20 characters
+2. contains the username string within the password
+3. Does not contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character (!, @, #, $, %, ^, &amp;, *, £)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+in the registration section of the Student Registration Page and click on the Register button..</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I Enter either "blank username" or "an already existing username" in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button on the student registration page of anodiam.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Invalid password. Password must be 8 to 20 characters long, must not contain your username and must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character (!, @, #, $, %, ^, &amp;, *, £)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter invalid email address
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. Does not contain exactly one '@' character.
+2. Does not contain one or more '.' characters after the '@' character.
+3. Does not contain any alphabet (a-z, A-Z) before '@'.
+4. Does not contain any alphabet (a-z, A-Z) in between '@' and '.'.
+5. Does not contain any alphabet (a-z, A-Z) after the last '.' character.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>in the registration section of the Student Registration Page and click on the Register button..</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter an already existing Anodiam username in the registration section of the Student Registration Page and click on the Register button..</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Invalid email address</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I Enter either "blank username" or "an already existing username" in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button on the student registration page of anodiam.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Invalid email address</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter already existing Anodiam user email address in the registration section of the Student Registration Page and click on the Register button..</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email address already exists</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I Enter either "blank username" or "an already existing username" in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button on the student registration page of anodiam.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email address already exists</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fill up the username and password fields with invalid username or password in the login page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Login </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve"> I am an unsigned but registered user
 </t>
     </r>
@@ -3203,8 +3928,130 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> I should be able to view the Anodiam Student Home Page: containing a welcome message with my (first and last) name at the top, a menu bar and a paginated list of courses recommended for me according to my Board, and Class, sans the courses I have already subscribed for (purchased), order by rating and total number of students. On wron userid or password I must be sent back to the login page with a login validation message (wrong user id or password) displayed on top in red</t>
-    </r>
+      <t xml:space="preserve"> I should be able to view the Anodiam Student Home Page: containing a welcome message with my (first and last) name at the top.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned but registered user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I fill up the username and password fields in the login page and click on the Login button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should be not able to view the Anodiam Student Home Page. Upon eneteing wrong userid or password I must be sent back to the login page with a login validation message (wrong user id or password) displayed on top in red</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I can not log in to anodiam.com and view the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student Home</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Upon eneteing wrong userid or password I must be sent back to the login page with a login validation message (wrong user id or password) displayed on top in red.</t>
+    </r>
+  </si>
+  <si>
+    <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Email Verification of student registration</t>
+  </si>
+  <si>
+    <t>Enabler</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>User registration fields (username, password, email) may contain personal information and must be encrypted at rest and inflight at all times</t>
+  </si>
+  <si>
+    <t>Cyber Security, Non-negotiable</t>
   </si>
 </sst>
 </file>
@@ -3291,7 +4138,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3307,6 +4154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3366,7 +4219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3414,6 +4267,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3425,6 +4279,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3659,31 +4525,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="A2" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -3754,25 +4620,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="56.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -3798,7 +4664,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>22</v>
@@ -3819,419 +4685,541 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:13" s="18" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="26">
+        <v>2</v>
+      </c>
+      <c r="J2" s="27">
+        <v>5</v>
+      </c>
+      <c r="K2" s="28">
+        <f t="shared" ref="K2:K19" si="0">IF(I2=0,0,J2/I2)</f>
+        <v>2.5</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="18" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="26">
+        <v>2</v>
+      </c>
+      <c r="J3" s="27">
+        <v>5</v>
+      </c>
+      <c r="K3" s="28">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M3" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="26">
+        <v>5</v>
+      </c>
+      <c r="J4" s="27">
+        <v>5</v>
+      </c>
+      <c r="K4" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M4" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26">
+        <v>3</v>
+      </c>
+      <c r="J5" s="27">
+        <v>5</v>
+      </c>
+      <c r="K5" s="28">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M5" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>3.2</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="26">
+        <v>3</v>
+      </c>
+      <c r="J6" s="27">
+        <v>5</v>
+      </c>
+      <c r="K6" s="28">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M6" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>3.3</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="26">
+        <v>3</v>
+      </c>
+      <c r="J7" s="27">
+        <v>5</v>
+      </c>
+      <c r="K7" s="28">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M7" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="19" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>3.4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="26">
+        <v>3</v>
+      </c>
+      <c r="J8" s="27">
+        <v>5</v>
+      </c>
+      <c r="K8" s="28">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M8" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="19" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="26">
+        <v>3</v>
+      </c>
+      <c r="J9" s="27">
+        <v>5</v>
+      </c>
+      <c r="K9" s="28">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M9" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>3.6</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="26">
+        <v>3</v>
+      </c>
+      <c r="J10" s="27">
+        <v>5</v>
+      </c>
+      <c r="K10" s="28">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M10" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>4</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="F11" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="26">
+        <v>2</v>
+      </c>
+      <c r="J11" s="27">
+        <v>5</v>
+      </c>
+      <c r="K11" s="28">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M11" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="25">
+        <v>5</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="26">
+        <v>5</v>
+      </c>
+      <c r="J12" s="27">
+        <v>5</v>
+      </c>
+      <c r="K12" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M12" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="26">
+        <v>5</v>
+      </c>
+      <c r="J13" s="27">
+        <v>5</v>
+      </c>
+      <c r="K13" s="28">
+        <f t="shared" ref="K13" si="1">IF(I13=0,0,J13/I13)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="10">
+      <c r="E14" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7">
+        <v>13</v>
+      </c>
+      <c r="J14" s="10">
         <v>5</v>
       </c>
-      <c r="K2" s="11">
-        <f t="shared" ref="K2" si="0">IF(I2=0,0,J2/I2)</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="K14" s="11">
+        <f>IF(I14=0,0,J14/I14)</f>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" s="18" customFormat="1" ht="229.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" s="18" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" s="18" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" s="18" customFormat="1" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>15</v>
@@ -4240,29 +5228,32 @@
         <v>16</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
+      <c r="K15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" s="18" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>15</v>
@@ -4271,29 +5262,32 @@
         <v>16</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="11"/>
+      <c r="K16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>15</v>
@@ -4302,29 +5296,32 @@
         <v>16</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="11"/>
+      <c r="K17" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>15</v>
@@ -4333,29 +5330,32 @@
         <v>16</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="11"/>
+      <c r="K18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>15</v>
@@ -4364,29 +5364,32 @@
         <v>16</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="11"/>
+      <c r="K19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:13" s="18" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>15</v>
@@ -4395,19 +5398,19 @@
         <v>16</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="10"/>
@@ -4415,9 +5418,9 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>15</v>
@@ -4426,19 +5429,19 @@
         <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="10"/>
@@ -4446,9 +5449,9 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>15</v>
@@ -4457,19 +5460,19 @@
         <v>16</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="10"/>
@@ -4477,9 +5480,9 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" s="18" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>15</v>
@@ -4488,19 +5491,19 @@
         <v>16</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="10"/>
@@ -4508,9 +5511,9 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" s="18" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>15</v>
@@ -4519,19 +5522,19 @@
         <v>16</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="10"/>
@@ -4539,9 +5542,9 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>15</v>
@@ -4550,19 +5553,19 @@
         <v>16</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="10"/>
@@ -4570,9 +5573,9 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>15</v>
@@ -4581,19 +5584,19 @@
         <v>16</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="10"/>
@@ -4601,9 +5604,9 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>15</v>
@@ -4612,19 +5615,19 @@
         <v>16</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="10"/>
@@ -4632,9 +5635,9 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="18" customFormat="1" ht="318.75" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>15</v>
@@ -4643,19 +5646,19 @@
         <v>16</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="10"/>
@@ -4663,9 +5666,9 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>15</v>
@@ -4674,19 +5677,19 @@
         <v>16</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="10"/>
@@ -4696,7 +5699,7 @@
     </row>
     <row r="30" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>15</v>
@@ -4705,19 +5708,19 @@
         <v>16</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="10"/>
@@ -4725,9 +5728,9 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="18" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>15</v>
@@ -4736,19 +5739,19 @@
         <v>16</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="10"/>
@@ -4756,35 +5759,283 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+    <row r="32" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>24</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="I32" s="7"/>
       <c r="J32" s="10"/>
       <c r="K32" s="11"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+    <row r="33" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>25</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="I33" s="7"/>
       <c r="J33" s="10"/>
       <c r="K33" s="11"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>26</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>27</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>28</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" s="7"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>29</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>30</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>31</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+    </row>
+    <row r="41" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1">
@@ -4793,19 +6044,19 @@
     </sortState>
   </autoFilter>
   <dataValidations xWindow="1023" yWindow="304" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J41">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L41">
       <formula1>"Initial,Scheduled,WIP,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I41">
       <formula1>"1,2,3,5,8,13"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B41">
       <formula1>"Feature,Enabler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C41">
       <formula1>"Epic,Story"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Product Backlog updated with no copy paste in password fields
29/10/2021
</commit_message>
<xml_diff>
--- a/ITProjectManagement/BA/SpecsWireframes/MVP/005MVPProductBacklog.xlsx
+++ b/ITProjectManagement/BA/SpecsWireframes/MVP/005MVPProductBacklog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="MVPProductBacklog" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MVPProductBacklog!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MVPProductBacklog!$A$1:$M$43</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="163">
   <si>
     <t>Anodiam</t>
   </si>
@@ -4196,6 +4196,140 @@
         <family val="2"/>
       </rPr>
       <t>Invalid password. Password must be 8 to 20 characters long, must not contain your username and must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
+    </r>
+  </si>
+  <si>
+    <t>Try to copy or paste in the Password field of the Login page</t>
+  </si>
+  <si>
+    <t>Try to copy or paste in the Password or Confirm Pasword fields of the Registration page</t>
+  </si>
+  <si>
+    <t>I am not allowed to Copy or paste in the Password field of the Login page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Try to copy or paste in the Password or Confirm Pasword fields of the Registration page.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am not allowed to Copy or paste in the Password or Confirm Pasword fields of the Registration page.</t>
+    </r>
+  </si>
+  <si>
+    <t>I am not allowed to Copy or paste in the Password or Confirm Pasword fields of the Registration page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Try to copy or paste in the Password field of the Login page.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am not allowed to Copy or paste in the Password field of the Login page.</t>
     </r>
   </si>
 </sst>
@@ -4364,7 +4498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4426,6 +4560,7 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4671,31 +4806,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -4766,11 +4901,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4863,7 +4998,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="24">
-        <f t="shared" ref="K2:K21" si="0">IF(I2=0,0,J2/I2)</f>
+        <f t="shared" ref="K2:K23" si="0">IF(I2=0,0,J2/I2)</f>
         <v>2.5</v>
       </c>
       <c r="L2" s="21" t="s">
@@ -5245,269 +5380,277 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
+    <row r="12" spans="1:13" s="25" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
+      <c r="K12" s="11">
+        <f>IF(I12=0,0,J12/I12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" s="25" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="7">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11">
+        <f>IF(I13=0,0,J13/I13)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
         <v>4</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G14" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I14" s="22">
         <v>2</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J14" s="23">
         <v>5</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K14" s="24">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L14" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M14" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+    <row r="15" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="21">
         <v>5</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B15" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E15" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G15" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I15" s="22">
         <v>5</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J15" s="23">
         <v>5</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K15" s="24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L15" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M15" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+    <row r="16" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C16" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E16" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F16" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G16" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I16" s="22">
         <v>5</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J16" s="23">
         <v>5</v>
       </c>
-      <c r="K14" s="24">
-        <f t="shared" ref="K14" si="1">IF(I14=0,0,J14/I14)</f>
+      <c r="K16" s="24">
+        <f t="shared" ref="K16" si="1">IF(I16=0,0,J16/I16)</f>
         <v>1</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L16" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M16" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+    <row r="17" spans="1:13" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>6</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7">
         <v>13</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J17" s="10">
         <v>5</v>
       </c>
-      <c r="K15" s="11">
-        <f>IF(I15=0,0,J15/I15)</f>
+      <c r="K17" s="11">
+        <f>IF(I17=0,0,J17/I17)</f>
         <v>0.38461538461538464</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>6.2</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7">
-        <v>5</v>
-      </c>
-      <c r="J16" s="10">
-        <v>1</v>
-      </c>
-      <c r="K16" s="11">
-        <f>IF(I16=0,0,J16/I16)</f>
-        <v>0.2</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>7</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>8</v>
-      </c>
-      <c r="B18" s="7" t="s">
+        <v>6.2</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="10"/>
+        <v>136</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7">
+        <v>5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>1</v>
+      </c>
       <c r="K18" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(I18=0,0,J18/I18)</f>
+        <v>0.2</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>15</v>
@@ -5519,16 +5662,16 @@
         <v>36</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="10"/>
@@ -5539,9 +5682,9 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>15</v>
@@ -5553,16 +5696,16 @@
         <v>36</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="10"/>
@@ -5575,7 +5718,7 @@
     </row>
     <row r="21" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>15</v>
@@ -5587,13 +5730,13 @@
         <v>36</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>43</v>
@@ -5607,9 +5750,9 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>15</v>
@@ -5621,26 +5764,29 @@
         <v>36</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="11"/>
+      <c r="K22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>15</v>
@@ -5652,26 +5798,29 @@
         <v>36</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="10"/>
-      <c r="K23" s="11"/>
+      <c r="K23" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>15</v>
@@ -5683,13 +5832,13 @@
         <v>36</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>51</v>
@@ -5700,9 +5849,9 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>15</v>
@@ -5714,16 +5863,16 @@
         <v>36</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="10"/>
@@ -5731,9 +5880,9 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>15</v>
@@ -5745,16 +5894,16 @@
         <v>36</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="10"/>
@@ -5762,9 +5911,9 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>15</v>
@@ -5776,16 +5925,16 @@
         <v>36</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="10"/>
@@ -5793,9 +5942,9 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>15</v>
@@ -5807,16 +5956,16 @@
         <v>36</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="10"/>
@@ -5824,9 +5973,9 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>15</v>
@@ -5838,16 +5987,16 @@
         <v>36</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="10"/>
@@ -5855,9 +6004,9 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" s="18" customFormat="1" ht="318.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>15</v>
@@ -5869,16 +6018,16 @@
         <v>36</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="10"/>
@@ -5886,9 +6035,9 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>15</v>
@@ -5900,16 +6049,16 @@
         <v>36</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="10"/>
@@ -5917,9 +6066,9 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="18" customFormat="1" ht="318.75" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>15</v>
@@ -5931,13 +6080,13 @@
         <v>36</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>85</v>
@@ -5948,9 +6097,9 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="1:13" s="18" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>15</v>
@@ -5962,13 +6111,13 @@
         <v>36</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>85</v>
@@ -5979,9 +6128,9 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>15</v>
@@ -5993,13 +6142,13 @@
         <v>36</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>85</v>
@@ -6010,9 +6159,9 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="18" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>15</v>
@@ -6024,13 +6173,13 @@
         <v>36</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>85</v>
@@ -6041,9 +6190,9 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>15</v>
@@ -6055,13 +6204,13 @@
         <v>36</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>85</v>
@@ -6072,9 +6221,9 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>15</v>
@@ -6086,13 +6235,13 @@
         <v>36</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>85</v>
@@ -6103,9 +6252,9 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>15</v>
@@ -6117,13 +6266,13 @@
         <v>36</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>85</v>
@@ -6136,7 +6285,7 @@
     </row>
     <row r="39" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>15</v>
@@ -6148,13 +6297,13 @@
         <v>36</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>85</v>
@@ -6167,7 +6316,7 @@
     </row>
     <row r="40" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>15</v>
@@ -6179,13 +6328,13 @@
         <v>36</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>85</v>
@@ -6196,9 +6345,9 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>15</v>
@@ -6210,13 +6359,13 @@
         <v>36</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>85</v>
@@ -6227,56 +6376,118 @@
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+    <row r="42" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>30</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I42" s="7"/>
       <c r="J42" s="10"/>
       <c r="K42" s="11"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+    <row r="43" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>31</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I43" s="7"/>
       <c r="J43" s="10"/>
       <c r="K43" s="11"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
     </row>
+    <row r="44" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+    </row>
+    <row r="45" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M1">
+  <autoFilter ref="A1:M43">
     <sortState ref="A2:O24">
       <sortCondition ref="K1"/>
     </sortState>
   </autoFilter>
   <dataValidations xWindow="1023" yWindow="304" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J45">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L45">
       <formula1>"Initial,Scheduled,WIP,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I45">
       <formula1>"1,2,3,5,8,13"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B45">
       <formula1>"Feature,Enabler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C45">
       <formula1>"Epic,Story"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Error messages updated in MVP Prod Backlog
11/11/2021
</commit_message>
<xml_diff>
--- a/ITProjectManagement/BA/SpecsWireframes/MVP/005MVPProductBacklog.xlsx
+++ b/ITProjectManagement/BA/SpecsWireframes/MVP/005MVPProductBacklog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="MVPProductBacklog" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MVPProductBacklog!$A$1:$M$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MVPProductBacklog!$A$1:$M$47</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="183">
   <si>
     <t>Anodiam</t>
   </si>
@@ -331,30 +331,6 @@
   </si>
   <si>
     <t>004MVPStudentAppWireframes.pptx &gt;&gt; Student Registration Page</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">I can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>register myself</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> as a student with anodiam.com</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2958,76 +2934,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">I cannot </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>register myself</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Invalid email address</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">I cannot </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>register myself</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Email address already exists</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Fill up the username and password fields with invalid username or password in the login page and click on the </t>
     </r>
     <r>
@@ -3241,188 +3147,6 @@
   </si>
   <si>
     <t>Enter already existing Anodiam user email address in the registration section of the Student Registration Page and click on the Register button.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am an unsigned user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I Enter either "blank username" or "an already existing username" in the registration section of the Student Registration Page and click on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Register </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">button
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Invalid email address</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am an unsigned user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I enter an already existing username in the Student Registration Page and click on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Register </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">button
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Email address already exists</t>
-    </r>
   </si>
   <si>
     <r>
@@ -3578,98 +3302,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am an unsigned user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I enter  invalid username (Less than 8 characters long or 
-an already existing username) in the registration section of the Student Registration Page and click on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Register </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">button
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Username cannot be less than 8 characters long</t>
-    </r>
-  </si>
-  <si>
     <t>Enter invalid username
 (Less than 8 characters long)
 in the registration section of the Student Registration Page and click on the Register button.</t>
@@ -3678,112 +3310,10 @@
     <t>Enter an already existing Anodiam username in the registration section of the Student Registration Page and click on the Register button.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">I </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>cannot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>register myself</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> as a student with anodiam.com. I must receive error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Username cannot be less than 8 characters</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">I </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>cannot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>register myself</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> as a student with anodiam.com. I must receive error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Username already exists</t>
-    </r>
+    <t>I cannot register myself as a student with anodiam.com. I must receive following error message: Password and Confirm Password fields do not match.</t>
+  </si>
+  <si>
+    <t>Enter wrong Confirm Password in the Student Registration Page and click on the Register button.</t>
   </si>
   <si>
     <r>
@@ -3823,8 +3353,177 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> I enter  invalid username (Less than 8 characters long or 
-an already existing username) in the registration section of the Student Registration Page and click on the </t>
+      <t xml:space="preserve"> I enter wrong Confirm Password in the Student Registration Page and click on the Register button.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Password and Confirm Password fields do not match.</t>
+    </r>
+  </si>
+  <si>
+    <t>Try to copy or paste in the Password field of the Login page</t>
+  </si>
+  <si>
+    <t>Try to copy or paste in the Password or Confirm Pasword fields of the Registration page</t>
+  </si>
+  <si>
+    <t>I am not allowed to Copy or paste in the Password field of the Login page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Try to copy or paste in the Password or Confirm Pasword fields of the Registration page.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am not allowed to Copy or paste in the Password or Confirm Pasword fields of the Registration page.</t>
+    </r>
+  </si>
+  <si>
+    <t>I am not allowed to Copy or paste in the Password or Confirm Pasword fields of the Registration page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Try to copy or paste in the Password field of the Login page.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am not allowed to Copy or paste in the Password field of the Login page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fill up all the fields: (username, password, confirm password, email) (all mandatory) with valid informations in the registration section of the Student Registration Page and click on the </t>
     </r>
     <r>
       <rPr>
@@ -3843,251 +3542,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">button
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Username already exists.</t>
-    </r>
-  </si>
-  <si>
-    <t>I cannot register myself as a student with anodiam.com. I must receive following error message: Password and Confirm Password fields do not match.</t>
-  </si>
-  <si>
-    <t>Enter wrong Confirm Password in the Student Registration Page and click on the Register button.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am an unsigned user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I enter wrong Confirm Password in the Student Registration Page and click on the Register button.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Password and Confirm Password fields do not match.</t>
-    </r>
-  </si>
-  <si>
-    <t>Try to copy or paste in the Password field of the Login page</t>
-  </si>
-  <si>
-    <t>Try to copy or paste in the Password or Confirm Pasword fields of the Registration page</t>
-  </si>
-  <si>
-    <t>I am not allowed to Copy or paste in the Password field of the Login page</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am an unsigned user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Try to copy or paste in the Password or Confirm Pasword fields of the Registration page.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am not allowed to Copy or paste in the Password or Confirm Pasword fields of the Registration page.</t>
-    </r>
-  </si>
-  <si>
-    <t>I am not allowed to Copy or paste in the Password or Confirm Pasword fields of the Registration page</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am an unsigned user
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>When</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Try to copy or paste in the Password field of the Login page.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> I am not allowed to Copy or paste in the Password field of the Login page.</t>
-    </r>
+      <t>button.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.4.1</t>
   </si>
   <si>
     <r>
@@ -4102,9 +3561,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>1. Less than 8 characters or more than 20 characters
-2. contains the username string or email string within the password
-3. Does not contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
+      <t>Less than 8 characters</t>
     </r>
     <r>
       <rPr>
@@ -4149,7 +3606,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Invalid password. Password must be 8 to 20 characters long, must not contain your username or email and must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
+      <t>Student registration failure! Invalid password. Password should be 8 to 20 characters long.</t>
     </r>
   </si>
   <si>
@@ -4190,11 +3647,1042 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve"> I enter  invalid password </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Less than 8 characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+in the registration section of the Student Registration Page and click on the Register button.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid password. Password should be 8 to 20 characters long.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.4.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter  invalid password </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>More than 20 characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+in the registration section of the Student Registration Page and click on the Register button.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid password. Password should be 8 to 20 characters long.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter invalid password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>More than 20 characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+in the registration section of the Student Registration Page and click on the Register button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enter invalid password that</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> contains the username string within the password </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>in the registration section of the Student Registration Page and click on the Register button.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. Upon successful registration, I get a  message on top of the registration page saying </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration successful!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I fill up all the fields: (username, password, confirm password, email) (all mandatory) in the registration section of the Student Registration Page with valid inputs and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should be able to register myself as a student with anodiam.com. Upon successful registration, I get a  message on top of the registration page saying </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration successful!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>cannot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! This username is already taken by another user. Please try some other username.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter  invalid username (an already existing username) in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! This username is already taken by another user. Please try some other username.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>Enter blank username
+in the registration section of the Student Registration Page and click on the Register button.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>cannot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Username should be 8 or more characters long.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter  invalid username (Less than 8 characters long) in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Username should be 8 or more characters long.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>cannot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Username cannot be blank.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter blank username in the registration section of the Student Registration Page and click on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Register </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Username cannot be blank.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid password. Password should not contain your username.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter  invalid password that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">contains the username string within the password </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">in the registration section of the Student Registration Page and click on the Register button.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid password. Password should not contain your username.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter invalid password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Does not contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+in the registration section of the Student Registration Page and click on the Register button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid password. Password must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z),at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve"> I enter  invalid password
-1. Less than 8 characters or more than 20 characters
-2. contains the username string  or email string within the password
-3. Does not contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)
-in the registration section of the Student Registration Page and click on the Register button.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Does not contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">in the registration section of the Student Registration Page and click on the Register button.
 </t>
     </r>
     <r>
@@ -4225,12 +4713,89 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Invalid password. Password must be 8 to 20 characters long, must not contain your username or email and must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z), at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fill up all the fields: (username, password, confirm password, email) (all mandatory) with valid informations in the registration section of the Student Registration Page and click on the </t>
+      <t>Student registration failure! Invalid password. Password must contain at least one small alphabet (a-z), at least one capital alphabet (A-Z),at least one numeric (0-9) and at least one special character among (@,#,$,%,^,&amp;,+,=)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid email address.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I am an unsigned user
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>When</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I enter invalid email address
+1. Does not contain exactly one '@' character.
+2. Does not contain one or more '.' characters after the '@' character.
+3. Does not contain any alphabet (a-z, A-Z) before '@'.
+4. Does not contain any alphabet (a-z, A-Z) in between '@' and '.'.
+5. Does not contain any alphabet (a-z, A-Z) after the last '.' character
+in the registration section of the Student Registration Page and click on the </t>
     </r>
     <r>
       <rPr>
@@ -4249,7 +4814,73 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>button.</t>
+      <t xml:space="preserve">button
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! Invalid email address</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I cannot </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>register myself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as a student with anodiam.com. I must receive following error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! An user with the same email address is already registered.</t>
     </r>
   </si>
   <si>
@@ -4290,7 +4921,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> I fill up all the fields: (username, password, confirm password, email) (all mandatory) in the registration section of the Student Registration Page and click on the </t>
+      <t xml:space="preserve"> I enter an already existing username in the Student Registration Page and click on the </t>
     </r>
     <r>
       <rPr>
@@ -4329,8 +4960,31 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> I should be able to register myself as a student with anodiam.com. Upon successful registration, I get a  message on top of the registration page saying "Registration Succesful".</t>
-    </r>
+      <t xml:space="preserve"> I should not be able to register myself as a student with anodiam.com. I should receive respective error message:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Student registration failure! An user with the same email address is already registered.</t>
+    </r>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>3.3.3</t>
+  </si>
+  <si>
+    <t>3.3.4</t>
   </si>
 </sst>
 </file>
@@ -4417,7 +5071,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4439,12 +5093,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4567,6 +5215,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4578,9 +5227,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4815,31 +5461,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -4910,11 +5556,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4954,7 +5600,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>22</v>
@@ -4986,16 +5632,16 @@
         <v>16</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>25</v>
@@ -5007,11 +5653,11 @@
         <v>5</v>
       </c>
       <c r="K2" s="24">
-        <f t="shared" ref="K2:K23" si="0">IF(I2=0,0,J2/I2)</f>
+        <f t="shared" ref="K2:K27" si="0">IF(I2=0,0,J2/I2)</f>
         <v>2.5</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M2" s="21">
         <v>1</v>
@@ -5028,16 +5674,16 @@
         <v>16</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" s="22" t="s">
         <v>25</v>
@@ -5053,13 +5699,13 @@
         <v>5</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M3" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -5070,16 +5716,16 @@
         <v>16</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>161</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>162</v>
       </c>
       <c r="H4" s="22" t="s">
         <v>26</v>
@@ -5095,7 +5741,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M4" s="21">
         <v>1</v>
@@ -5106,7 +5752,7 @@
         <v>3.1</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>16</v>
@@ -5114,10 +5760,10 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="22">
@@ -5131,15 +5777,15 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M5" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="21">
-        <v>3.2</v>
+    <row r="6" spans="1:13" s="19" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>15</v>
@@ -5148,40 +5794,40 @@
         <v>16</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>143</v>
+        <v>166</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="H6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I6" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" s="23">
         <v>5</v>
       </c>
       <c r="K6" s="24">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M6" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
-        <v>3.3</v>
+    <row r="7" spans="1:13" s="19" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>15</v>
@@ -5190,40 +5836,40 @@
         <v>16</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>148</v>
+        <v>162</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>163</v>
       </c>
       <c r="H7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="23">
         <v>5</v>
       </c>
       <c r="K7" s="24">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M7" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="19" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
-        <v>3.4</v>
+    <row r="8" spans="1:13" s="26" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>15</v>
@@ -5232,40 +5878,40 @@
         <v>16</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>160</v>
+        <v>168</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>169</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" s="23">
         <v>5</v>
       </c>
       <c r="K8" s="24">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <f t="shared" ref="K8" si="1">IF(I8=0,0,J8/I8)</f>
+        <v>2.5</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M8" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="19" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21">
-        <v>3.5</v>
+    <row r="9" spans="1:13" s="26" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>179</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>15</v>
@@ -5274,40 +5920,40 @@
         <v>16</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>138</v>
+        <v>152</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>153</v>
       </c>
       <c r="H9" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I9" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="23">
         <v>5</v>
       </c>
       <c r="K9" s="24">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <f t="shared" ref="K9" si="2">IF(I9=0,0,J9/I9)</f>
+        <v>2.5</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M9" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="19" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
-        <v>3.6</v>
+    <row r="10" spans="1:13" s="26" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>15</v>
@@ -5316,40 +5962,40 @@
         <v>16</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>139</v>
+        <v>152</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="23">
         <v>5</v>
       </c>
       <c r="K10" s="24">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <f t="shared" ref="K10" si="3">IF(I10=0,0,J10/I10)</f>
+        <v>2.5</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M10" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="20" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="21">
-        <v>3.7</v>
+    <row r="11" spans="1:13" s="26" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>181</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>15</v>
@@ -5358,16 +6004,16 @@
         <v>16</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>151</v>
+        <v>170</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>171</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>26</v>
@@ -5376,22 +6022,22 @@
         <v>2</v>
       </c>
       <c r="J11" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K11" s="24">
-        <f>IF(I11=0,0,J11/I11)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>129</v>
+        <f t="shared" ref="K11" si="4">IF(I11=0,0,J11/I11)</f>
+        <v>2.5</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="M11" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="25" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
-        <v>3.8</v>
+    <row r="12" spans="1:13" s="26" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>182</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>15</v>
@@ -5400,16 +6046,16 @@
         <v>16</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>155</v>
+        <v>173</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>174</v>
       </c>
       <c r="H12" s="22" t="s">
         <v>26</v>
@@ -5418,22 +6064,22 @@
         <v>2</v>
       </c>
       <c r="J12" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K12" s="24">
-        <f>IF(I12=0,0,J12/I12)</f>
-        <v>0.5</v>
+        <f t="shared" ref="K12" si="5">IF(I12=0,0,J12/I12)</f>
+        <v>2.5</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M12" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="25" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
-        <v>3.8</v>
+    <row r="13" spans="1:13" s="19" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>15</v>
@@ -5442,58 +6088,58 @@
         <v>16</v>
       </c>
       <c r="D13" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>152</v>
-      </c>
       <c r="F13" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>157</v>
+        <v>175</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="22">
         <v>2</v>
       </c>
       <c r="J13" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K13" s="24">
-        <f>IF(I13=0,0,J13/I13)</f>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M13" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
-        <v>4</v>
-      </c>
-      <c r="B14" s="22" t="s">
+    <row r="14" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>30</v>
+        <v>177</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>26</v>
@@ -5509,301 +6155,333 @@
         <v>2.5</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M14" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="20" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
+        <v>3.5</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="22">
+        <v>2</v>
+      </c>
+      <c r="J15" s="23">
+        <v>3</v>
+      </c>
+      <c r="K15" s="24">
+        <f>IF(I15=0,0,J15/I15)</f>
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="M15" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="25" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
+        <v>3.6</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="22">
+        <v>2</v>
+      </c>
+      <c r="J16" s="23">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24">
+        <f>IF(I16=0,0,J16/I16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M16" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="25" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="21">
+        <v>3.7</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="22">
+        <v>2</v>
+      </c>
+      <c r="J17" s="23">
+        <v>1</v>
+      </c>
+      <c r="K17" s="24">
+        <f>IF(I17=0,0,J17/I17)</f>
+        <v>0.5</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
+        <v>4</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="22">
+        <v>2</v>
+      </c>
+      <c r="J18" s="23">
         <v>5</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="K18" s="24">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M18" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
+        <v>5</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="H15" s="22" t="s">
+      <c r="D19" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I19" s="22">
         <v>5</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J19" s="23">
         <v>5</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K19" s="24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L19" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M19" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="22">
+        <v>5</v>
+      </c>
+      <c r="J20" s="23">
+        <v>5</v>
+      </c>
+      <c r="K20" s="24">
+        <f t="shared" ref="K20" si="6">IF(I20=0,0,J20/I20)</f>
+        <v>1</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="M20" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="M15" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="19" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="21">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="G16" s="22" t="s">
+      <c r="D21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="22">
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
+        <v>13</v>
+      </c>
+      <c r="J21" s="10">
         <v>5</v>
       </c>
-      <c r="J16" s="23">
-        <v>5</v>
-      </c>
-      <c r="K16" s="24">
-        <f t="shared" ref="K16" si="1">IF(I16=0,0,J16/I16)</f>
-        <v>1</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="M16" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>6</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7">
-        <v>13</v>
-      </c>
-      <c r="J17" s="10">
-        <v>5</v>
-      </c>
-      <c r="K17" s="11">
-        <f>IF(I17=0,0,J17/I17)</f>
+      <c r="K21" s="11">
+        <f>IF(I21=0,0,J21/I21)</f>
         <v>0.38461538461538464</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>6.2</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7">
-        <v>5</v>
-      </c>
-      <c r="J18" s="10">
-        <v>1</v>
-      </c>
-      <c r="K18" s="11">
-        <f>IF(I18=0,0,J18/I18)</f>
-        <v>0.2</v>
-      </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>8</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>9</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>10</v>
-      </c>
-      <c r="B22" s="7" t="s">
+        <v>6.2</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="10"/>
+        <v>133</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7">
+        <v>5</v>
+      </c>
+      <c r="J22" s="10">
+        <v>1</v>
+      </c>
       <c r="K22" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(I22=0,0,J22/I22)</f>
+        <v>0.2</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>15</v>
@@ -5812,19 +6490,19 @@
         <v>16</v>
       </c>
       <c r="D23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="F23" s="7" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="10"/>
@@ -5835,9 +6513,9 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>15</v>
@@ -5846,29 +6524,32 @@
         <v>16</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="10"/>
-      <c r="K24" s="11"/>
+      <c r="K24" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>15</v>
@@ -5877,29 +6558,32 @@
         <v>16</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="10"/>
-      <c r="K25" s="11"/>
+      <c r="K25" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>15</v>
@@ -5908,29 +6592,32 @@
         <v>16</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="10"/>
-      <c r="K26" s="11"/>
+      <c r="K26" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>15</v>
@@ -5939,29 +6626,32 @@
         <v>16</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="11"/>
+      <c r="K27" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>15</v>
@@ -5970,19 +6660,19 @@
         <v>16</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="10"/>
@@ -5990,9 +6680,9 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>15</v>
@@ -6001,19 +6691,19 @@
         <v>16</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="10"/>
@@ -6021,9 +6711,9 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>15</v>
@@ -6032,19 +6722,19 @@
         <v>16</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="10"/>
@@ -6052,9 +6742,9 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>15</v>
@@ -6063,19 +6753,19 @@
         <v>16</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="10"/>
@@ -6083,9 +6773,9 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" s="18" customFormat="1" ht="318.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="18" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>15</v>
@@ -6094,19 +6784,19 @@
         <v>16</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="10"/>
@@ -6114,9 +6804,9 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>15</v>
@@ -6125,19 +6815,19 @@
         <v>16</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="10"/>
@@ -6147,7 +6837,7 @@
     </row>
     <row r="34" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>15</v>
@@ -6156,19 +6846,19 @@
         <v>16</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="10"/>
@@ -6176,9 +6866,9 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" s="18" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="18" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>15</v>
@@ -6187,19 +6877,19 @@
         <v>16</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="10"/>
@@ -6207,9 +6897,9 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="18" customFormat="1" ht="318.75" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>15</v>
@@ -6218,19 +6908,19 @@
         <v>16</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="10"/>
@@ -6240,7 +6930,7 @@
     </row>
     <row r="37" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>15</v>
@@ -6249,19 +6939,19 @@
         <v>16</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="10"/>
@@ -6269,9 +6959,9 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>15</v>
@@ -6280,19 +6970,19 @@
         <v>16</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="10"/>
@@ -6300,9 +6990,9 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" s="18" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>15</v>
@@ -6311,19 +7001,19 @@
         <v>16</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="10"/>
@@ -6331,9 +7021,9 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="18" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>15</v>
@@ -6342,19 +7032,19 @@
         <v>16</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="10"/>
@@ -6362,9 +7052,9 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>15</v>
@@ -6373,19 +7063,19 @@
         <v>16</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="10"/>
@@ -6393,9 +7083,9 @@
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>15</v>
@@ -6404,19 +7094,19 @@
         <v>16</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="10"/>
@@ -6424,9 +7114,9 @@
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>15</v>
@@ -6435,19 +7125,19 @@
         <v>16</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="10"/>
@@ -6455,56 +7145,180 @@
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
+    <row r="44" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <v>28</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="I44" s="7"/>
       <c r="J44" s="10"/>
       <c r="K44" s="11"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+    <row r="45" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>29</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="I45" s="7"/>
       <c r="J45" s="10"/>
       <c r="K45" s="11"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
     </row>
+    <row r="46" spans="1:13" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>30</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="7"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="1:13" s="18" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>31</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I47" s="7"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M43">
+  <autoFilter ref="A1:M47">
     <sortState ref="A2:O24">
       <sortCondition ref="K1"/>
     </sortState>
   </autoFilter>
   <dataValidations xWindow="1023" yWindow="304" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Business Value Error!" error="Business Value should be an integer between 1 to 5!" sqref="J2:J49">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error!" error="Please select Status only from the dropdown!!!" sqref="L2:L49">
       <formula1>"Initial,Scheduled,WIP,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estimates Error!" error="Enter Story Points in Fibonacci!!!" promptTitle="Enter Story Points in Fibonacci" prompt="Enter Story Points in Fibonacci Series: 1, 2, 3, 5, 8, 13." sqref="I2:I49">
       <formula1>"1,2,3,5,8,13"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B49">
       <formula1>"Feature,Enabler"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C49">
       <formula1>"Epic,Story"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>